<commit_message>
parser must be configured + various refactoring
</commit_message>
<xml_diff>
--- a/spring-projects/src/test/resources/com/github/vincent_fuchs/spring_projects/excelReader/simpleInputFile.xlsx
+++ b/spring-projects/src/test/resources/com/github/vincent_fuchs/spring_projects/excelReader/simpleInputFile.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="customer" sheetId="1" r:id="rId1"/>
+    <sheet name="customers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -376,7 +376,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding a second worksheet and parsing it as well
</commit_message>
<xml_diff>
--- a/spring-projects/src/test/resources/com/github/vincent_fuchs/spring_projects/excelReader/simpleInputFile.xlsx
+++ b/spring-projects/src/test/resources/com/github/vincent_fuchs/spring_projects/excelReader/simpleInputFile.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="1" r:id="rId1"/>
+    <sheet name="addresses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Id</t>
   </si>
@@ -32,6 +33,30 @@
   </si>
   <si>
     <t>age</t>
+  </si>
+  <si>
+    <t>customerId</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>expectedStreet</t>
+  </si>
+  <si>
+    <t>expectedCIty</t>
+  </si>
+  <si>
+    <t>expectedCountry</t>
   </si>
 </sst>
 </file>
@@ -375,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -412,4 +437,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
committed from GSC premises - test
</commit_message>
<xml_diff>
--- a/spring-projects/src/test/resources/com/github/vincent_fuchs/spring_projects/excelReader/simpleInputFile.xlsx
+++ b/spring-projects/src/test/resources/com/github/vincent_fuchs/spring_projects/excelReader/simpleInputFile.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="customers" sheetId="1" r:id="rId1"/>
     <sheet name="addresses" sheetId="2" r:id="rId2"/>
+    <sheet name="test" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -62,8 +63,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -154,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,10 +187,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,7 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,16 +396,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -440,16 +439,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -466,7 +465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -486,4 +485,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>